<commit_message>
ajout d'une url pour la commission
</commit_message>
<xml_diff>
--- a/src/main/resources/template/exports-xlsx/commissions_template.xlsx
+++ b/src/main/resources/template/exports-xlsx/commissions_template.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kevin\Desktop\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="1890" yWindow="4185" windowWidth="18555" windowHeight="5610"/>
   </bookViews>
@@ -14,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
   <si>
     <t>Libelle</t>
   </si>
@@ -146,12 +151,24 @@
   </si>
   <si>
     <t>${membre.profil}&lt;/jt:forEach&gt;</t>
+  </si>
+  <si>
+    <t>Url</t>
+  </si>
+  <si>
+    <t>${com.url}</t>
+  </si>
+  <si>
+    <t>${com.temShowMail}</t>
+  </si>
+  <si>
+    <t>Affichage mail</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -215,7 +232,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -226,6 +243,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -241,6 +264,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -289,7 +315,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -324,7 +350,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -533,11 +559,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U4"/>
+  <dimension ref="A1:W4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -547,30 +573,32 @@
     <col min="4" max="4" width="12" style="3" customWidth="1"/>
     <col min="5" max="5" width="29.5703125" style="3" customWidth="1"/>
     <col min="6" max="6" width="24.7109375" style="3" customWidth="1"/>
-    <col min="7" max="7" width="26.140625" style="3" customWidth="1"/>
-    <col min="8" max="8" width="30" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="20.28515625" style="3" customWidth="1"/>
-    <col min="11" max="11" width="23" style="3" customWidth="1"/>
-    <col min="12" max="12" width="37.28515625" style="3" customWidth="1"/>
-    <col min="13" max="13" width="27.140625" style="3" customWidth="1"/>
-    <col min="14" max="14" width="33.28515625" style="3" customWidth="1"/>
-    <col min="15" max="15" width="21.28515625" style="3" customWidth="1"/>
-    <col min="16" max="16" width="23.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="27" style="3" customWidth="1"/>
-    <col min="18" max="18" width="24.5703125" style="3" customWidth="1"/>
-    <col min="19" max="19" width="17.7109375" style="3" customWidth="1"/>
-    <col min="20" max="20" width="25.140625" style="3" customWidth="1"/>
-    <col min="21" max="21" width="26.140625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="19.5703125" style="3" customWidth="1"/>
+    <col min="8" max="8" width="24.7109375" style="3" customWidth="1"/>
+    <col min="9" max="9" width="26.140625" style="3" customWidth="1"/>
+    <col min="10" max="10" width="30" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="20.28515625" style="3" customWidth="1"/>
+    <col min="13" max="13" width="23" style="3" customWidth="1"/>
+    <col min="14" max="14" width="37.28515625" style="3" customWidth="1"/>
+    <col min="15" max="15" width="27.140625" style="3" customWidth="1"/>
+    <col min="16" max="16" width="33.28515625" style="3" customWidth="1"/>
+    <col min="17" max="17" width="21.28515625" style="3" customWidth="1"/>
+    <col min="18" max="18" width="23.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="27" style="3" customWidth="1"/>
+    <col min="20" max="20" width="24.5703125" style="3" customWidth="1"/>
+    <col min="21" max="21" width="17.7109375" style="3" customWidth="1"/>
+    <col min="22" max="22" width="25.140625" style="3" customWidth="1"/>
+    <col min="23" max="23" width="26.140625" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:23" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="8"/>
+      <c r="C1" s="10"/>
       <c r="D1" s="4" t="s">
         <v>2</v>
       </c>
@@ -580,60 +608,66 @@
       <c r="F1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="I1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="J1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="K1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="L1" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="M1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="N1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="O1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="P1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="Q1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="R1" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="Q1" s="4" t="s">
+      <c r="S1" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="R1" s="4" t="s">
+      <c r="T1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="S1" s="4" t="s">
+      <c r="U1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="T1" s="4" t="s">
+      <c r="V1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="U1" s="4" t="s">
+      <c r="W1" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:21" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:23" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="9"/>
+      <c r="C2" s="11"/>
       <c r="D2" s="2" t="s">
         <v>22</v>
       </c>
@@ -644,52 +678,58 @@
         <v>24</v>
       </c>
       <c r="G2" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="I2" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="K2" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="L2" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="M2" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="N2" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="O2" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="N2" s="2" t="s">
+      <c r="P2" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="O2" s="2" t="s">
+      <c r="Q2" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="P2" s="2" t="s">
+      <c r="R2" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="Q2" s="2" t="s">
+      <c r="S2" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="R2" s="2" t="s">
+      <c r="T2" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="S2" s="2" t="s">
+      <c r="U2" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="T2" s="2" t="s">
+      <c r="V2" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="U2" s="2" t="s">
+      <c r="W2" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:23" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
         <v>41</v>
       </c>
@@ -702,8 +742,8 @@
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
       <c r="F3" s="7"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
       <c r="I3" s="5"/>
       <c r="J3" s="5"/>
       <c r="K3" s="5"/>
@@ -716,11 +756,13 @@
       <c r="R3" s="5"/>
       <c r="S3" s="5"/>
       <c r="T3" s="5"/>
-      <c r="U3" s="2" t="s">
+      <c r="U3" s="5"/>
+      <c r="V3" s="5"/>
+      <c r="W3" s="2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:21" s="3" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="4" spans="1:23" s="3" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="B1:C1"/>

</xml_diff>

<commit_message>
ajout d'un mail d'alerte pour la commission
</commit_message>
<xml_diff>
--- a/src/main/resources/template/exports-xlsx/commissions_template.xlsx
+++ b/src/main/resources/template/exports-xlsx/commissions_template.xlsx
@@ -159,10 +159,10 @@
     <t>${com.url}</t>
   </si>
   <si>
-    <t>${com.temShowMail}</t>
-  </si>
-  <si>
-    <t>Affichage mail</t>
+    <t>Mail alerte</t>
+  </si>
+  <si>
+    <t>${com.mailAlert}</t>
   </si>
 </sst>
 </file>
@@ -561,9 +561,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H8" sqref="H8"/>
+      <selection pane="bottomLeft" activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -572,12 +572,10 @@
     <col min="2" max="3" width="29" style="3" customWidth="1"/>
     <col min="4" max="4" width="12" style="3" customWidth="1"/>
     <col min="5" max="5" width="29.5703125" style="3" customWidth="1"/>
-    <col min="6" max="6" width="24.7109375" style="3" customWidth="1"/>
-    <col min="7" max="7" width="19.5703125" style="3" customWidth="1"/>
-    <col min="8" max="8" width="24.7109375" style="3" customWidth="1"/>
-    <col min="9" max="9" width="26.140625" style="3" customWidth="1"/>
-    <col min="10" max="10" width="30" style="3" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="20.28515625" style="3" customWidth="1"/>
+    <col min="6" max="7" width="24.7109375" style="3" customWidth="1"/>
+    <col min="8" max="8" width="26.140625" style="3" customWidth="1"/>
+    <col min="9" max="9" width="30" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="12" width="20.28515625" style="3" customWidth="1"/>
     <col min="13" max="13" width="23" style="3" customWidth="1"/>
     <col min="14" max="14" width="37.28515625" style="3" customWidth="1"/>
     <col min="15" max="15" width="27.140625" style="3" customWidth="1"/>
@@ -608,23 +606,23 @@
       <c r="F1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="H1" s="8" t="s">
+      <c r="G1" s="8" t="s">
         <v>44</v>
       </c>
+      <c r="H1" s="4" t="s">
+        <v>9</v>
+      </c>
       <c r="I1" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="L1" s="4" t="s">
         <v>17</v>
+      </c>
+      <c r="L1" s="9" t="s">
+        <v>46</v>
       </c>
       <c r="M1" s="4" t="s">
         <v>12</v>
@@ -678,22 +676,22 @@
         <v>24</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>45</v>
+        <v>25</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>29</v>
+        <v>47</v>
       </c>
       <c r="M2" s="2" t="s">
         <v>30</v>
@@ -743,7 +741,7 @@
       <c r="E3" s="6"/>
       <c r="F3" s="7"/>
       <c r="G3" s="7"/>
-      <c r="H3" s="7"/>
+      <c r="H3" s="5"/>
       <c r="I3" s="5"/>
       <c r="J3" s="5"/>
       <c r="K3" s="5"/>

</xml_diff>